<commit_message>
Added UI and inventory
Added UI and all it's functionalities, equiping items, switch
characters. Implemented inventory to be easilly used with the inventory
user interface
</commit_message>
<xml_diff>
--- a/Hours.xlsx
+++ b/Hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Setting up and analyzing syndicate game</t>
   </si>
@@ -35,6 +35,15 @@
   </si>
   <si>
     <t xml:space="preserve">Figger out how to best use required class structure </t>
+  </si>
+  <si>
+    <t>Setting up the ui dynamically and making it organized</t>
+  </si>
+  <si>
+    <t>Setting up inventory, easilly adding/removing item's and displaying them correctly</t>
+  </si>
+  <si>
+    <t>Using ui to influence gameplay: equip item's switch character</t>
   </si>
 </sst>
 </file>
@@ -376,15 +385,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.75" customWidth="1"/>
+    <col min="1" max="1" width="62.125" customWidth="1"/>
     <col min="2" max="2" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -444,6 +453,30 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added enemy's, persuading, itemdrops
Added enemy's that shoot back and can kill players, persuading enemy's
to join and follow you, dropping of items when killing an enemy and
picking them up by walking over it.
</commit_message>
<xml_diff>
--- a/Hours.xlsx
+++ b/Hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Setting up and analyzing syndicate game</t>
   </si>
@@ -44,6 +44,30 @@
   </si>
   <si>
     <t>Using ui to influence gameplay: equip item's switch character</t>
+  </si>
+  <si>
+    <t>Enhancements</t>
+  </si>
+  <si>
+    <t>Hud</t>
+  </si>
+  <si>
+    <t>Follow/Remain Button</t>
+  </si>
+  <si>
+    <t>Persuading an enemy to follow you</t>
+  </si>
+  <si>
+    <t>Enemy shoot back when syndicate's gun out and are in tange</t>
+  </si>
+  <si>
+    <t>Enemy drop random items you pick up by walking over them</t>
+  </si>
+  <si>
+    <t>Spawn enemy's at random position</t>
+  </si>
+  <si>
+    <t>15min</t>
   </si>
 </sst>
 </file>
@@ -385,16 +409,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.125" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,6 +501,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added objective and pedestrians
Added a goal to the level and pedestrians who walk arround
</commit_message>
<xml_diff>
--- a/Hours.xlsx
+++ b/Hours.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Setting up and analyzing syndicate game</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>15min</t>
+  </si>
+  <si>
+    <t>Pedestrians</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Task:</t>
+  </si>
+  <si>
+    <t>Hours:</t>
   </si>
 </sst>
 </file>
@@ -409,53 +421,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -463,7 +475,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>0.5</v>
@@ -471,7 +483,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -479,31 +491,31 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -511,7 +523,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -519,23 +531,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -543,18 +555,42 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>